<commit_message>
Tests for elo calculation
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfprysl/workspace/elo_oim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE801D4E-BE0E-354A-A667-152569F5B78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42E10BC-25D9-7145-BE3C-9721D84E2328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="2" xr2:uid="{AA925308-2E72-A94B-A7EE-22B3B6643D21}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="5" xr2:uid="{AA925308-2E72-A94B-A7EE-22B3B6643D21}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Ranks" sheetId="5" r:id="rId5"/>
     <sheet name="Calculations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -156,7 +156,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -175,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +194,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -207,18 +213,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -238,10 +249,7 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -311,12 +319,12 @@
   <autoFilter ref="A1:G5" xr:uid="{288F00DA-98D9-9F4C-B751-1152884F1374}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{1E50419C-6445-8146-8E74-63F299DD865B}" name="Player"/>
-    <tableColumn id="2" xr3:uid="{57DA1B97-4BE6-5540-B45F-E7EDD9CDE57A}" name="Start" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{265D07B1-32D3-224A-AFA4-5C59250978D2}" name="Game1" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{39F592F3-44E1-964B-8EF4-3D1636EFC5A5}" name="Game2" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A98FBF95-BE59-7F48-9258-1D82C91EA3B1}" name="Game3" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{C1F1F770-756E-0144-B0AF-44B6DC0FFA6E}" name="Game4" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{CACE2A4C-4005-A846-B953-4943F6EA6083}" name="Game5" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{57DA1B97-4BE6-5540-B45F-E7EDD9CDE57A}" name="Start" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{265D07B1-32D3-224A-AFA4-5C59250978D2}" name="Game1" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{39F592F3-44E1-964B-8EF4-3D1636EFC5A5}" name="Game2" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{A98FBF95-BE59-7F48-9258-1D82C91EA3B1}" name="Game3" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{C1F1F770-756E-0144-B0AF-44B6DC0FFA6E}" name="Game4" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{CACE2A4C-4005-A846-B953-4943F6EA6083}" name="Game5" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -326,7 +334,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B005885D-449D-E741-9D2E-55C35C3760D8}" name="Score6" displayName="Score6" ref="A1:L6" totalsRowShown="0">
   <autoFilter ref="A1:L6" xr:uid="{DD564CFA-CBAB-F64F-8346-E37273E5E05C}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{D57FA753-59FA-014F-A452-D8372D9FA5EB}" name="Timestamp" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{D57FA753-59FA-014F-A452-D8372D9FA5EB}" name="Timestamp" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{BB3277FF-99AC-C44A-987D-64528710C50A}" name="Tournament"/>
     <tableColumn id="3" xr3:uid="{40C26732-F407-F943-B6BD-52538F235502}" name="Player1"/>
     <tableColumn id="4" xr3:uid="{37D9CD8A-571E-C545-BE04-47A853149980}" name="Army1"/>
@@ -754,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2558315B-4006-4F4E-A3D5-5788CFF8D163}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1147,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{594204D6-A8C7-624C-BAB5-4A2F52F03012}">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1376,40 +1384,40 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="6">
         <v>45845.541666666664</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="7">
         <v>7</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="7">
         <v>8</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="7">
         <v>3</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="7">
         <v>1</v>
       </c>
       <c r="N4" s="3">
@@ -1600,6 +1608,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
     <ignoredError sqref="S4:T4 S5" formula="1"/>
   </ignoredErrors>

</xml_diff>